<commit_message>
Excels corregidos espacios quitados en proyectos de tls 201812 y 201811
</commit_message>
<xml_diff>
--- a/Excels/Proyectos Informacionales.xlsx
+++ b/Excels/Proyectos Informacionales.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cperezin\everis\BBVA Gestión - Documentos\1.General Datos Económicos\11.Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmartino\Desktop\PruebasBlackMargin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6440"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>EXT-000193-00895</t>
   </si>
@@ -246,19 +246,34 @@
   </si>
   <si>
     <t>Recuperaciones</t>
+  </si>
+  <si>
+    <t>EXT-000193-00894</t>
+  </si>
+  <si>
+    <t>DNA AM:POC MICRO FY '18'</t>
+  </si>
+  <si>
+    <t>AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -315,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -324,6 +339,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -801,29 +819,27 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>0</v>
+    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>65</v>
@@ -831,13 +847,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>65</v>
@@ -845,41 +861,41 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>55</v>
@@ -887,47 +903,47 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
@@ -938,10 +954,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>67</v>
@@ -951,36 +967,50 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>29</v>
+      <c r="A25" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -989,6 +1019,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AC7593AF650CCD4DA29693C434D9B93D" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="87b01934b614e4f37b4d036e08def249">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c5c0a092-86e7-4d19-9228-f591611b7342" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c60d6c4eb9101f020e3664cd21a59f74" ns2:_="">
     <xsd:import namespace="c5c0a092-86e7-4d19-9228-f591611b7342"/>
@@ -1120,29 +1165,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAB93D87-CC78-43A3-8F80-F4B3E5C61EC3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{908436A3-98DD-4E13-A3AE-AA0EBB0921A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D89E-643E-40E6-9D9A-421A5DCAFB0E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D89E-643E-40E6-9D9A-421A5DCAFB0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{908436A3-98DD-4E13-A3AE-AA0EBB0921A9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAB93D87-CC78-43A3-8F80-F4B3E5C61EC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c5c0a092-86e7-4d19-9228-f591611b7342"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
corregido espacio en xlsx de TLS201810 y añadida descripcion de proyecto al Ext-000193-00907
</commit_message>
<xml_diff>
--- a/Excels/Proyectos Informacionales.xlsx
+++ b/Excels/Proyectos Informacionales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmartino\Desktop\PruebasBlackMargin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmartino\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t>EXT-000193-00895</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>AM</t>
+  </si>
+  <si>
+    <t>Pool Visualizacion</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -919,6 +922,9 @@
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>55</v>
@@ -1019,18 +1025,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1166,18 +1172,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{908436A3-98DD-4E13-A3AE-AA0EBB0921A9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D89E-643E-40E6-9D9A-421A5DCAFB0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D89E-643E-40E6-9D9A-421A5DCAFB0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{908436A3-98DD-4E13-A3AE-AA0EBB0921A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Últimas modificaciones del proyecto MarginBlack
</commit_message>
<xml_diff>
--- a/Excels/Proyectos Informacionales.xlsx
+++ b/Excels/Proyectos Informacionales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruizarr\Documents\Margin\MarginBlack\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmartino\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t>EXT-000193-00895</t>
   </si>
@@ -258,22 +258,25 @@
   </si>
   <si>
     <t>Pool Visualizacion</t>
-  </si>
-  <si>
-    <t>BICC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -330,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -339,6 +342,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,8 +822,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -836,7 +842,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>65</v>
@@ -919,9 +925,7 @@
       <c r="B21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>55</v>
       </c>
@@ -948,7 +952,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>67</v>
@@ -962,7 +966,7 @@
         <v>48</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>67</v>
@@ -976,7 +980,7 @@
         <v>49</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>67</v>

</xml_diff>